<commit_message>
add Excel sheet with RADLEX terms
</commit_message>
<xml_diff>
--- a/fileRIDs.xlsx
+++ b/fileRIDs.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B188"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,31 +560,31 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/070.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/132.xml</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID49834</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/132.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/251.xml</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834</t>
+          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/251.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/285.xml</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -596,43 +596,43 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/187/285.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/001.xml</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/001.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/099.xml</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID3875, RID38780, RID49834</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/099.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/120.xml</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RID5998, RID3875, RID38780, RID49834</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/120.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/055.xml</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -644,31 +644,31 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/055.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/125.xml</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID49834</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/125.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/143.xml</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834</t>
+          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/143.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/157.xml</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -680,139 +680,139 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/157.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/142.xml</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998, RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/189/142.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/175.xml</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/175.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/202.xml</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/202.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/204.xml</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID49834</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/204.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/060.xml</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/060.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/066.xml</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/066.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/138.xml</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/138.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/110.xml</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/110.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/044.xml</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RID5998</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/044.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/130.xml</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/130.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/157.xml</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/157.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/220.xml</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -824,67 +824,67 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/220.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/018.xml</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780, RID49834</t>
+          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/018.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/187.xml</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID3875, RID38780</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/187.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/033.xml</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/033.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/153.xml</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RID5998, RID49834, RID3875, RID38780</t>
+          <t>RID5998, RID3875, RID38780, RID49834</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/188/153.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/162.xml</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>RID5998, RID3875, RID38780, RID49834</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/162.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/176.xml</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -896,19 +896,19 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/176.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/189.xml</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/189.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/201.xml</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -920,55 +920,55 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/201.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/215.xml</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/215.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/163.xml</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/163.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/014.xml</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/014.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/202.xml</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/202.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/148.xml</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -980,19 +980,19 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/148.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/158.xml</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/158.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/170.xml</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1004,31 +1004,31 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/170.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/164.xml</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/164.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/207.xml</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/207.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/159.xml</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1040,43 +1040,43 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/159.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/205.xml</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/205.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/204.xml</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/204.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/172.xml</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/172.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/166.xml</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/166.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/101.xml</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1100,31 +1100,31 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/101.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/115.xml</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/115.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/263.xml</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/263.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/060.xml</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1136,19 +1136,19 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/060.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/289.xml</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/289.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/100.xml</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1160,7 +1160,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/100.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/275.xml</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1172,31 +1172,31 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/275.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/271.xml</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/271.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/067.xml</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/067.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/066.xml</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1208,43 +1208,43 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/066.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/112.xml</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/112.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/104.xml</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/104.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/110.xml</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/110.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/299.xml</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1256,7 +1256,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/299.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/058.xml</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/058.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/267.xml</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1280,19 +1280,19 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/267.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/105.xml</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/105.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/139.xml</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1304,31 +1304,31 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/139.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/256.xml</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/256.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/082.xml</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/082.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/069.xml</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1340,7 +1340,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/069.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/280.xml</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1352,7 +1352,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/280.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/243.xml</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1364,79 +1364,79 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/243.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/241.xml</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/241.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/255.xml</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/255.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/296.xml</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/296.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/043.xml</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/043.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/240.xml</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/240.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/122.xml</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/122.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/136.xml</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1448,43 +1448,43 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/136.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/132.xml</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/132.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/278.xml</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/278.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/085.xml</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/085.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/292.xml</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/292.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/286.xml</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1508,19 +1508,19 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/286.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/245.xml</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/245.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/253.xml</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/253.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/290.xml</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1544,43 +1544,43 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/290.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/087.xml</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/087.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/044.xml</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/044.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/050.xml</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/050.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/285.xml</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1592,7 +1592,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/285.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/252.xml</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1604,43 +1604,43 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/252.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/180.xml</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/180.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/194.xml</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/194.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/209.xml</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/209.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/037.xml</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1652,31 +1652,31 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/037.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/234.xml</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/234.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/236.xml</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/236.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/008.xml</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/008.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/196.xml</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1700,7 +1700,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/196.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/145.xml</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1712,67 +1712,67 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/145.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/227.xml</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/227.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/150.xml</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/150.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/178.xml</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/178.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/033.xml</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/033.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/219.xml</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/219.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/190.xml</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1784,7 +1784,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/186/190.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/189.xml</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1796,7 +1796,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/189.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/214.xml</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -1808,19 +1808,19 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/214.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/202.xml</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/202.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/158.xml</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1832,55 +1832,55 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/158.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/164.xml</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/164.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/213.xml</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/213.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/173.xml</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/173.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/239.xml</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/239.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/075.xml</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -1892,7 +1892,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/075.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/289.xml</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -1904,7 +1904,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/289.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/276.xml</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -1916,55 +1916,55 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/276.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/128.xml</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/128.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/114.xml</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/114.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/116.xml</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID29, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/116.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/260.xml</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29, RID3875, RID38780</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/260.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/274.xml</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -1976,31 +1976,31 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/274.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/249.xml</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/249.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/261.xml</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/261.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/271.xml</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2012,7 +2012,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/271.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/099.xml</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2024,7 +2024,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/099.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/264.xml</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2036,31 +2036,31 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/264.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/112.xml</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/112.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/104.xml</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/104.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/070.xml</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2072,79 +2072,79 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/070.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/267.xml</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/267.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/273.xml</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/273.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/120.xml</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/120.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/256.xml</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/256.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/068.xml</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/068.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/294.xml</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/294.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/109.xml</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -2156,7 +2156,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/109.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/135.xml</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/135.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/241.xml</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2180,7 +2180,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/241.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/269.xml</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -2192,7 +2192,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/269.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/095.xml</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/095.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/297.xml</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -2216,55 +2216,55 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/297.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/268.xml</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/268.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/254.xml</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>RID5998, RID5689, RID45847, RID49834, RID3875, RID38780</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/254.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/122.xml</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/122.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/132.xml</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/132.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/084.xml</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -2276,19 +2276,19 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/084.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/292.xml</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/292.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/247.xml</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -2300,19 +2300,19 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/247.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/290.xml</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/290.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/284.xml</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -2324,7 +2324,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/284.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/093.xml</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -2336,7 +2336,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/093.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/124.xml</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/124.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/180.xml</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -2360,31 +2360,31 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/180.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/235.xml</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/235.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/181.xml</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/181.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/183.xml</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -2396,7 +2396,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/183.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/182.xml</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -2408,43 +2408,43 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/182.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/196.xml</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/196.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/141.xml</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>RID5689, RID45847</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/141.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/179.xml</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/179.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/186.xml</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -2456,31 +2456,31 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/186.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/227.xml</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/227.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/232.xml</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/232.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/185.xml</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -2492,118 +2492,106 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/185.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/219.xml</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID5689, RID45847, RID29</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/219.xml</t>
+          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/184.xml</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID29</t>
+          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>LIDC-IDRI/LIDC-IDRI_RadiologistAnnotationsSegmentations/tcia-lidc-xml/185/184.xml</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_omf_v4.0_sarc.txt</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>RID5689, RID45847, RID3875, RID38780, RID29</t>
+          <t>RID49815, RID8, RID36042, RID5821, RID3957, RID1560</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_omf_v4.0_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_nte_sarc.txt</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID36042, RID5821, RID3957, RID1560</t>
+          <t>RID49815, RID5720, RID3957, RID1560, RID38780, RID34301, RID39123, RID39144, RID39066, RID35973, RID39068, RID28492, RID5727, RID39330, RID5972, RID5703, RID8, RID1559, RID58</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_nte_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_nte_sarc.txt</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>RID49815, RID5720, RID3957, RID1560, RID38780, RID34301, RID39123, RID39144, RID39066, RID35973, RID39068, RID28492, RID5727, RID39330, RID5972, RID5703, RID8, RID1559, RID58</t>
+          <t>RID49815, RID5703, RID28492, RID3957, RID5720, RID1560, RID38780, RID34301, RID39123, RID39144, RID39066, RID35973, RID5727, RID39330, RID5972, RID39068, RID8, RID7741, RID5833, RID1301, RID28474</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_nte_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_radiation_sarc.txt</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>RID49815, RID5703, RID28492, RID3957, RID5720, RID1560, RID38780, RID34301, RID39123, RID39144, RID39066, RID35973, RID5727, RID39330, RID5972, RID39068, RID8, RID1559, RID7741, RID5833, RID1301, RID28474</t>
+          <t>RID49815, RID8, RID10409, RID49442, RID49572, RID3957, RID11515, RID39162, RID46056</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_radiation_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_sarc.txt</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID10409, RID49442, RID49572, RID3957, RID11515, RID39162, RID46056</t>
+          <t>RID49815, RID8, RID35973, RID3957, RID34658, RID5720, RID5729, RID34616, RID5655, RID46056, RID5689, RID45847, RID11514, RID5734, RID28474, RID11515, RID39162</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_follow_up_v4.0_sarc.txt</t>
+          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_drug_sarc.txt</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>RID49815, RID8, RID35973, RID3957, RID34658, RID5720, RID5729, RID34616, RID5655, RID46056, RID5689, RID45847, RID11514, RID5734, RID28474, RID11515, RID39162</t>
+          <t>RID49815, RID35973, RID8, RID28492, RID10409, RID49442</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>TCGA-SARC/TCGA-SARC_ClinicalData/TCGA-SARC_nationwidechildrens.org_clinical_drug_sarc.txt</t>
+          <t>NSCLC-Radiomics-Interobserver1/NSCLC-Radiomics-Interobserver1_ClinicalData.csv</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
-        <is>
-          <t>RID49815, RID35973, RID8, RID28492, RID10409, RID49442</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>NSCLC-Radiomics-Interobserver1/NSCLC-Radiomics-Interobserver1_ClinicalData.csv</t>
-        </is>
-      </c>
-      <c r="B188" t="inlineStr">
         <is>
           <t>RID5653, RID4226, RID5825, RID5974, RID5967, RID39348, RID4247, RID5824, RID5962, RID5654, RID5774, RID1301, RID34616, RID46057, RID5778, RID46058</t>
         </is>

</xml_diff>